<commit_message>
book do projeto feito
</commit_message>
<xml_diff>
--- a/Book/Sprint 1/Product_Backlog.xlsx
+++ b/Book/Sprint 1/Product_Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SPTECH\SEGUNDO SEMESTRE\PROJETO\TEP\Book\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5D6F85-68A1-4B2F-8C4D-46B9D7A09DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408C81F2-10B0-4CC4-B128-AEF50A1532D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{590B817E-873B-4BA3-9FB9-EEA9816A006D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{590B817E-873B-4BA3-9FB9-EEA9816A006D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="136">
   <si>
     <t>Cadastro na Web</t>
   </si>
@@ -372,24 +372,6 @@
     <t>Semana 1 – Semana 4</t>
   </si>
   <si>
-    <t>- Cadastro Web</t>
-  </si>
-  <si>
-    <t>- Site Institucional com DataViz</t>
-  </si>
-  <si>
-    <t>- Estrutura inicial do BD</t>
-  </si>
-  <si>
-    <t>- Configuração de ambiente (Linux, Acesso remoto, GitHub, Planner)</t>
-  </si>
-  <si>
-    <t>- Primeiros gráficos (Dispersão, Barras, Pizza)</t>
-  </si>
-  <si>
-    <t>- Documentação inicial</t>
-  </si>
-  <si>
     <t>RF01, RF02, RF03, RF03.1, RF03.2, RF03.3, RNF01, RNF02, RNF03, RNF04, RNF05, RNF06, RNF09, RNF13, RNF14</t>
   </si>
   <si>
@@ -399,27 +381,6 @@
     <t>Semana 5 – Semana 8</t>
   </si>
   <si>
-    <t>- Dashboard consolidado</t>
-  </si>
-  <si>
-    <t>- CRUDs completos</t>
-  </si>
-  <si>
-    <t>- KPIs principais</t>
-  </si>
-  <si>
-    <t>- Parametrização e envio de notificações</t>
-  </si>
-  <si>
-    <t>- Extração com ApachePOI</t>
-  </si>
-  <si>
-    <t>- Logs básicos</t>
-  </si>
-  <si>
-    <t>- Usabilidade/UX</t>
-  </si>
-  <si>
     <t>RF03.4, RF03.5, RF03.6, RF04, RF04.1, RF04.2, RF04.3, RF05, RF06, RF09, RF10, RNF08, RNF11, RNF12, RNF15</t>
   </si>
   <si>
@@ -429,28 +390,64 @@
     <t>Semana 9 – Semana 12</t>
   </si>
   <si>
-    <t>- Filtros por período</t>
-  </si>
-  <si>
-    <t>- Detalhes de município</t>
-  </si>
-  <si>
-    <t>- Atualização automática do dashboard</t>
-  </si>
-  <si>
-    <t>- Responsividade obrigatória</t>
-  </si>
-  <si>
-    <t>- Segurança IAM</t>
-  </si>
-  <si>
-    <t>- Dockerização + Deploy AWS</t>
-  </si>
-  <si>
-    <t>- Lições aprendidas finais</t>
-  </si>
-  <si>
     <t>RF11, RF12, RF13, RNF07, RNF10, RNF11, RNF12, RNF15,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wireframe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logs </t>
+  </si>
+  <si>
+    <t>Parametrização e envio de notificações</t>
+  </si>
+  <si>
+    <t>KPIs principais</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CRUDs completos</t>
+  </si>
+  <si>
+    <t>Dashboard consolidado</t>
+  </si>
+  <si>
+    <t>Documentação inicial</t>
+  </si>
+  <si>
+    <t>Configuração de ambiente (Linux, Acesso remoto, GitHub, Planner)</t>
+  </si>
+  <si>
+    <t>Estrutura inicial do BD</t>
+  </si>
+  <si>
+    <t>Site Institucional com DataViz</t>
+  </si>
+  <si>
+    <t>Logs básicos</t>
+  </si>
+  <si>
+    <t>Usabilidade/UX</t>
+  </si>
+  <si>
+    <t>Filtros por período</t>
+  </si>
+  <si>
+    <t>Detalhes de município</t>
+  </si>
+  <si>
+    <t>Atualização automática do dashboard</t>
+  </si>
+  <si>
+    <t>Responsividade obrigatória</t>
+  </si>
+  <si>
+    <t>Segurança IAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dockerização + Deploy AWS</t>
+  </si>
+  <si>
+    <t>Lições aprendidas finais</t>
   </si>
 </sst>
 </file>
@@ -530,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -548,17 +545,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -896,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F1E06F4-0190-49FD-AB20-FAF1B1527CEC}">
   <dimension ref="A1:W40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1945,8 +1945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2474D0A0-7946-473E-8594-632069213C95}">
   <dimension ref="B1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="53" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1959,196 +1959,196 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="8" t="s">
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" s="10"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" s="10"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" s="10"/>
+    </row>
+    <row r="12" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E12" s="10"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="10"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="D15" s="9" t="s">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="9"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9" t="s">
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9" t="s">
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="9"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9" t="s">
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="9"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9" t="s">
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9" t="s">
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E20" s="8"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="E21" s="8"/>
+      <c r="E21" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>